<commit_message>
Updated bench, last version
</commit_message>
<xml_diff>
--- a/BenchRSA(PyCryptoLib).xlsx
+++ b/BenchRSA(PyCryptoLib).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uninsubria365-my.sharepoint.com/personal/lerba_studenti_uninsubria_it/Documents/UNINSU/AppuntiTesi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo\Desktop\UNINSU\CryptoThesis\Commitment_Schemes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_AD4D5CB4E552A5DACE1C6466081D4A145ADEDD81" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADD89661-6F54-40A3-96E6-64B6EE91E9FB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8952E8-E8F1-431B-8E04-01A78C2C1DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -106,12 +106,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -398,21 +396,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.85546875" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="49.88671875" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" customWidth="1"/>
+    <col min="4" max="4" width="25.5546875" customWidth="1"/>
     <col min="5" max="5" width="38" customWidth="1"/>
-    <col min="6" max="6" width="43.85546875" customWidth="1"/>
+    <col min="6" max="6" width="43.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -426,7 +424,7 @@
         <v>13.8588376045227</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -446,92 +444,83 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3.38625907897949E-3</v>
       </c>
       <c r="B3" s="1">
         <v>7.0308446884155204E-2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>3.84183621406555</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
         <v>5.07354736328125E-4</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>1.06573104858398E-4</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="1">
         <v>0.38824510574340798</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3.2393932342529201E-3</v>
       </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3.1945705413818299E-3</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3.1628608703613199E-3</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4.6272277832031198E-3</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3.7841796875E-3</v>
       </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3.8797855377197201E-3</v>
       </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3.18026542663574E-3</v>
       </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3.19910049438476E-3</v>
       </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4.5380592346191398E-3</v>
       </c>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f>AVERAGE(A3:A12)</f>
         <v>3.6191701889038037E-3</v>
       </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -545,7 +534,7 @@
         <v>23.025265761099998</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f>AVERAGE(A3:A12)</f>
         <v>3.6191701889038037E-3</v>
@@ -566,7 +555,7 @@
         <v>1.2566223144531199</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -580,7 +569,7 @@
         <v>58.040489673614502</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f>AVERAGE(A3:A12)</f>
         <v>3.6191701889038037E-3</v>
@@ -588,7 +577,7 @@
       <c r="B20" s="1">
         <v>0.83</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="1">
         <v>46.536026999999997</v>
       </c>
       <c r="D20" s="1">
@@ -597,19 +586,11 @@
       <c r="E20" s="1">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="1">
         <v>4.55</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -623,15 +604,15 @@
         <v>121.259761095047</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f>AVERAGE(A3:A12)</f>
         <v>3.6191701889038037E-3</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="1">
         <v>1.79619288444519</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="2">
         <v>97.743110000000001</v>
       </c>
       <c r="D24" s="1">
@@ -644,7 +625,7 @@
         <v>9.6240599155426008</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -658,15 +639,15 @@
         <v>193.10640000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f>AVERAGE(A3:A12)</f>
         <v>3.6191701889038037E-3</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="1">
         <v>2.9823</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="2">
         <v>169.217706680297</v>
       </c>
       <c r="D29" s="1">
@@ -675,7 +656,7 @@
       <c r="E29" s="1">
         <v>3.7996768951415998E-3</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="2">
         <v>16.468016147613501</v>
       </c>
     </row>

</xml_diff>